<commit_message>
Check if the Sudoku is Legit
</commit_message>
<xml_diff>
--- a/sudoku.xlsx
+++ b/sudoku.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akifarslan/Desktop/Pyhton Projects/PyQt5_Study/Project_Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akifarslan/Desktop/Pyhton Projects/Sudoku-08-22-21/project_folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE05F017-796C-6747-919C-0F0D5EA8E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56635500-7173-A249-AF6D-ED008EAFBA0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -61,7 +61,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -326,11 +326,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -410,6 +488,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,13 +1110,15 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="200" zoomScaleNormal="188" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="192" zoomScaleNormal="188" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="2.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="2.33203125" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.33203125" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="4.5" style="2"/>
   </cols>
@@ -1043,11 +1131,11 @@
         <v>3</v>
       </c>
       <c r="C1" s="7"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1">
-        <v>7</v>
-      </c>
-      <c r="F1" s="14"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="6">
+        <v>7</v>
+      </c>
+      <c r="F1" s="40"/>
       <c r="G1" s="5"/>
       <c r="H1" s="6"/>
       <c r="I1" s="7"/>
@@ -1092,7 +1180,7 @@
       <c r="I3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="4">
+      <c r="A4" s="41">
         <v>8</v>
       </c>
       <c r="B4" s="4"/>
@@ -1104,12 +1192,12 @@
       <c r="F4" s="7"/>
       <c r="G4" s="18"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="4">
+      <c r="I4" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
       <c r="B5" s="1"/>
@@ -1123,12 +1211,12 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1"/>
-      <c r="I5" s="1">
+      <c r="I5" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="43">
         <v>7</v>
       </c>
       <c r="B6" s="16"/>
@@ -1140,7 +1228,7 @@
       <c r="F6" s="12"/>
       <c r="G6" s="15"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="16">
+      <c r="I6" s="44">
         <v>6</v>
       </c>
     </row>
@@ -1184,11 +1272,11 @@
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="12"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1">
-        <v>8</v>
-      </c>
-      <c r="F9" s="14"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="11">
+        <v>8</v>
+      </c>
+      <c r="F9" s="46"/>
       <c r="G9" s="10"/>
       <c r="H9" s="11">
         <v>7</v>
@@ -1200,31 +1288,31 @@
     <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B12" s="20">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C12" s="37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D12" s="19">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E12" s="20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F12" s="21">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G12" s="19">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H12" s="20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I12" s="21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>0</v>
@@ -1232,147 +1320,147 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B13" s="23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C13" s="24">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D13" s="25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E13" s="23">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F13" s="26">
         <v>5</v>
       </c>
       <c r="G13" s="25">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H13" s="23">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I13" s="26">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="38">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B14" s="31">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C14" s="32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D14" s="27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F14" s="29">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G14" s="27">
         <v>5</v>
       </c>
       <c r="H14" s="28">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I14" s="29">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B15" s="20">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C15" s="21">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D15" s="35">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E15" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F15" s="34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G15" s="19">
         <v>4</v>
       </c>
       <c r="H15" s="20">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I15" s="21">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="25">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B16" s="23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16" s="26">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D16" s="22">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F16" s="24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" s="25">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H16" s="23">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I16" s="26">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B17" s="28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C17" s="29">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D17" s="30">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E17" s="31">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F17" s="32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G17" s="27">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H17" s="28">
         <v>5</v>
       </c>
       <c r="I17" s="29">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1380,86 +1468,86 @@
         <v>9</v>
       </c>
       <c r="B18" s="20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E18" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="21">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G18" s="19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H18" s="20">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I18" s="21">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B19" s="23">
         <v>8</v>
       </c>
       <c r="C19" s="26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D19" s="25">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E19" s="23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F19" s="26">
         <v>9</v>
       </c>
       <c r="G19" s="25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H19" s="23">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I19" s="26">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="28">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C20" s="29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" s="27">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E20" s="28">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F20" s="29">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G20" s="27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H20" s="28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I20" s="29">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1474,7 +1562,7 @@
   <dimension ref="A1:AG20"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="125" workbookViewId="0">
-      <selection activeCell="V24" sqref="V24"/>
+      <selection sqref="A1:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>